<commit_message>
Add spawn enemies & Add colide
0613 Upload.
spawn enemies (normal, speed, gun, shield)
colide player with enemies / enemies with bullet

Todo: make Rpg's bomb.  gun enemy shot to player.
code rearrange.
</commit_message>
<xml_diff>
--- a/FinalProject/최종 시험-문제참고용.xlsx
+++ b/FinalProject/최종 시험-문제참고용.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJS\Desktop\Project\Infinite-War\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE106392-DB69-4144-A04B-FBBBCED2077F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEF31C2-8FB0-4445-962D-26F1A3C5A04C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="1080" windowWidth="20910" windowHeight="14325" xr2:uid="{CD1EEE43-91F0-4D97-8AA8-F6E7C9A3DE09}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD1EEE43-91F0-4D97-8AA8-F6E7C9A3DE09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>순번</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -821,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DA367B-150E-40A1-B4C5-3F6804069325}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1318,9 +1318,6 @@
       </c>
       <c r="D39">
         <v>5</v>
-      </c>
-      <c r="E39" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add Bomb, score, pause
Add Bomb, score, pause.
some code rearranged.
Linq, interface, out ... for score.

Todo : gun enemy shot to player. code rearrange.
</commit_message>
<xml_diff>
--- a/FinalProject/최종 시험-문제참고용.xlsx
+++ b/FinalProject/최종 시험-문제참고용.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJS\Desktop\Project\Infinite-War\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEF31C2-8FB0-4445-962D-26F1A3C5A04C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A04B8C1-F71E-417A-874A-5FB4BAEBF92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD1EEE43-91F0-4D97-8AA8-F6E7C9A3DE09}"/>
+    <workbookView xWindow="7170" yWindow="1725" windowWidth="20910" windowHeight="14325" xr2:uid="{CD1EEE43-91F0-4D97-8AA8-F6E7C9A3DE09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>순번</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -259,6 +259,10 @@
   </si>
   <si>
     <t>제네릭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쓸꺼임!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -821,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DA367B-150E-40A1-B4C5-3F6804069325}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -831,28 +835,28 @@
     <col min="2" max="2" width="72.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -863,7 +867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -877,7 +881,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -891,7 +895,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -905,7 +909,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
@@ -915,7 +919,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>53</v>
       </c>
@@ -925,7 +929,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -939,7 +943,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>2</v>
       </c>
@@ -950,7 +954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>3</v>
       </c>
@@ -964,7 +968,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>4</v>
       </c>
@@ -978,7 +982,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>5</v>
       </c>
@@ -989,14 +993,14 @@
         <v>-70</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>1</v>
       </c>
@@ -1006,8 +1010,14 @@
       <c r="C16" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>2</v>
       </c>
@@ -1021,7 +1031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>3</v>
       </c>
@@ -1035,7 +1045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>4</v>
       </c>
@@ -1049,7 +1059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>5</v>
       </c>
@@ -1063,7 +1073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>6</v>
       </c>
@@ -1074,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>7</v>
       </c>
@@ -1084,8 +1094,11 @@
       <c r="C22" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>8</v>
       </c>
@@ -1099,7 +1112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>9</v>
       </c>
@@ -1110,7 +1123,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>10</v>
       </c>
@@ -1124,7 +1137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>11</v>
       </c>
@@ -1138,7 +1151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>12</v>
       </c>
@@ -1152,7 +1165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>13</v>
       </c>
@@ -1163,7 +1176,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>14</v>
       </c>
@@ -1176,11 +1189,8 @@
       <c r="D29">
         <v>3</v>
       </c>
-      <c r="E29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>15</v>
       </c>
@@ -1194,7 +1204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>16</v>
       </c>
@@ -1208,7 +1218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>17</v>
       </c>
@@ -1344,6 +1354,9 @@
       <c r="C41" s="2">
         <v>3</v>
       </c>
+      <c r="D41">
+        <v>3</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
@@ -1355,6 +1368,9 @@
       <c r="C42" s="2">
         <v>5</v>
       </c>
+      <c r="D42">
+        <v>5</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
@@ -1366,6 +1382,9 @@
       <c r="C43" s="2">
         <v>8</v>
       </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
@@ -1377,6 +1396,9 @@
       <c r="C44" s="2">
         <v>4</v>
       </c>
+      <c r="D44">
+        <v>4</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
@@ -1388,6 +1410,9 @@
       <c r="C45" s="2">
         <v>5</v>
       </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
@@ -1468,7 +1493,7 @@
         <v>5</v>
       </c>
       <c r="D50">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E50" t="s">
         <v>56</v>
@@ -1485,7 +1510,7 @@
       </c>
       <c r="D51">
         <f>SUM(D16:D50)</f>
-        <v>66</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Sound, Sword, Pause, Record, GunEnemy, PlayerDie, Weapon cool
Last Algorithm Update. (Complete game)

Add Sound (BGM, Effect)
Update Sword structure
Add Pause system (ESC key)
Add Recording system.
Update GunEnemy (now, can shoot bullet for player)
Add PlayerDie (when die, esc to menu)
Add Showing Weapon cool.

Todo : Make PPT, Comment.
</commit_message>
<xml_diff>
--- a/FinalProject/최종 시험-문제참고용.xlsx
+++ b/FinalProject/최종 시험-문제참고용.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJS\Desktop\Project\Infinite-War\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A04B8C1-F71E-417A-874A-5FB4BAEBF92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA0EDE4-9CED-4979-9494-21130B9439F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7170" yWindow="1725" windowWidth="20910" windowHeight="14325" xr2:uid="{CD1EEE43-91F0-4D97-8AA8-F6E7C9A3DE09}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{CD1EEE43-91F0-4D97-8AA8-F6E7C9A3DE09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>순번</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -251,10 +251,6 @@
   </si>
   <si>
     <t>기본 점수 (30점 만점)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -825,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DA367B-150E-40A1-B4C5-3F6804069325}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1014,7 +1010,7 @@
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1175,6 +1171,9 @@
       <c r="C28" s="2">
         <v>3</v>
       </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
@@ -1232,7 +1231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>18</v>
       </c>
@@ -1246,7 +1245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>19</v>
       </c>
@@ -1260,7 +1259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>20</v>
       </c>
@@ -1274,7 +1273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>21</v>
       </c>
@@ -1288,7 +1287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>22</v>
       </c>
@@ -1302,7 +1301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>23</v>
       </c>
@@ -1316,7 +1315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>24</v>
       </c>
@@ -1330,7 +1329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>25</v>
       </c>
@@ -1344,7 +1343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>26</v>
       </c>
@@ -1358,7 +1357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>27</v>
       </c>
@@ -1372,7 +1371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>28</v>
       </c>
@@ -1386,7 +1385,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>29</v>
       </c>
@@ -1400,7 +1399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>30</v>
       </c>
@@ -1414,7 +1413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>31</v>
       </c>
@@ -1427,11 +1426,8 @@
       <c r="D46">
         <v>2</v>
       </c>
-      <c r="E46" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>32</v>
       </c>
@@ -1444,11 +1440,8 @@
       <c r="D47">
         <v>2</v>
       </c>
-      <c r="E47" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>33</v>
       </c>
@@ -1460,9 +1453,6 @@
       </c>
       <c r="D48">
         <v>2</v>
-      </c>
-      <c r="E48" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1478,9 +1468,6 @@
       <c r="D49">
         <v>2</v>
       </c>
-      <c r="E49" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
@@ -1496,7 +1483,7 @@
         <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1510,7 +1497,7 @@
       </c>
       <c r="D51">
         <f>SUM(D16:D50)</f>
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>